<commit_message>
agent integrated with places
</commit_message>
<xml_diff>
--- a/places.xlsx
+++ b/places.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,33 +487,53 @@
           <t>lead_score</t>
         </is>
       </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>ui_report</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>brief</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>pain_point_report</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>email_sample</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ChIJI5sPUzKTLoQR8MfAsEIA0YI</t>
+          <t>ChIJTcRk4PDIxokR7eKhkC6zST8</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Love &amp; Box</t>
+          <t>NJ Small Business Development Center @ Rutgers-Camden</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>gift_shop, point_of_interest, store, establishment</t>
+          <t>consultant, point_of_interest, establishment</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>(347) 831-0256</t>
+          <t>(856) 225-6221</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -522,58 +542,108 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>http://www.loveandbox.com/</t>
+          <t>http://rsbdc.org/</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://maps.google.com/?cid=9426315781496424432&amp;g_mp=Cidnb29nbGUubWFwcy5wbGFjZXMudjEuUGxhY2VzLlNlYXJjaFRleHQQAhgEIAA</t>
+          <t>https://maps.google.com/?cid=4560373110265733869&amp;g_mp=Cidnb29nbGUubWFwcy5wbGFjZXMudjEuUGxhY2VzLlNlYXJjaFRleHQQAhgEIAA</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>I bought a custom birthday gift for my best friend who already have everything.. And she just loved it!!
-Thank you Lara for the perfect and beautiful box.
-My friend got it right on time for the occasion.
-I highly recommend Love&amp;Box for the people you love. | I ordered a custom box as a gift for my mother-in-law who loves reading!! This is the perfect Reader’s Box! Absolutely beautiful and unique! Highly recommend Love&amp;Box for those special  gifts!! Thank you so much!!! | Beautiful unique personalized gifts, great selection, great service. I bought from them several times, for holidays and for baby. They shipped the gift promptly directly to the recipient.</t>
+          <t>Best Small Business resource available from idea to expansion and beyond ! | Very helpful and highly recommended for small business owners or those who wish to start a business | Info on help you start a business. 👍</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve">lara@loveandbox.com, </t>
+          <t>rsbdc@camden.rutgers.edu, ag2953@camden.rutgers.edu</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>4.15</v>
+        <v>2</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>**UI Improvements:**
+1. **Branding Inconsistency:**
+   - The Rutgers branding is strong in the header, but the use of different color palettes for SBDC, navigation, and titles introduces visual fragmentation. Keeping a unified color scheme would create a more cohesive brand experience.
+2. **Outdated Visual Style:**
+   - The design, with its heavy use of colored blocks and drop shadows, aligns more with early 2010s trends. Modern UIs emphasize flat design, subtle gradients, softer shadows, and more white space.
+   - Fonts look dated; consider using a modern, web-optimized font for body text (e.g., Inter, Roboto, Open Sans).
+3. **Navigation:**
+   - The horizontal navigation bar uses all-caps text, which can be harder to read and less accessible. Consider using sentence case or title case.
+   - The “COUNSELING REQUEST” button should stand out but feels visually disconnected from the navigation bar due to color and placement. Consistent button styles and better spacing would help.
+4. **Carousel/Slider:**
+   - The carousel area is mostly white space and lacks visual engagement. Text is hard to read due to low contrast against the background.
+   - Carousel arrows are too small/light — increase their size and contrast.
+   - If possible, add relevant imagery or background graphics to make this section more engaging.
+5. **Iconography and Cards:**
+   - The icons for Innovate/Launch/etc. are not visually aligned and seem mismatched in style.
+   - Card UI could benefit from increased padding, rounded corners, and more separation from the background to improve readability and touch-friendliness.
+6. **Sponsor Section:**
+   - Logos are unevenly scaled and not evenly spaced. Use consistent sizing and padding for a more polished appearance.
+   - Section title (“Annual Key Sponsors”) is not visually prominent—use more hierarchy to make it stand out.
+7. **Footer:**
+   - Contact info is usable but can be enhanced with clickable phone and email links.
+   - Section headers (“Contact Us,” “Rutgers University–Camden”) need better visual separation from the rest of the content.
+   - Consider using icons for contact methods.
+   - Footer background color would help differentiate it from main content.
+8. **Accessibility:**
+   - Text contrast could be improved in several areas (especially the carousel).
+   - Navigation should have visible focus states for keyboard users.
+   - Increase overall font size for body text and navigation.
+   - Ensure all actionable elements (e.g., buttons, links) meet minimum recommended tap/click sizes.
+9. **Responsiveness:**
+   - While screenshot doesn’t show mobile, ensure cards and navbar stack nicely on smaller screens, and legibility is retained.
+**Summary:**
+The site is functional but visually outdated, with branding inconsistencies, lack of modern UI polish, and several accessibility shortcomings. Updating to current UI trends, improving consistency, and enhancing accessibility would provide significant improvements.</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>**Business Context and Analysis:**  
+The NJ Small Business Development Center (NJSBDC) at Rutgers-Camden is a nonprofit resource center dedicated to supporting entrepreneurs and small business owners across Burlington, Camden, Gloucester, and Salem Counties in New Jersey. Operating under Rutgers University and partially funded by the SBA, the center provides no-cost consulting, business training workshops, and educational resources covering business planning, financing, marketing, certifications, e-business, and more. Their hybrid support model includes personalized consulting and group training, positioning them as a key catalyst for small business growth and local economic development.
+**Quick Wins &amp; Recommended Opportunities:**  
+Given the center's focus on education and outreach, implementing automated appointment scheduling, CRM for tracking client touchpoints, and online intake forms would streamline client engagement and improve operational efficiency. Website improvements could include a clearer call to action for service sign-ups, integration of live chat or chatbot support, and better organization of downloadable resources for quick access. Highlighting measurable client success stories and providing more intuitive navigation will further engage visitors and reinforce the SBDC’s impact. Additionally, reviewing back-office workflows for automation (e.g., training registration, event reminders, and feedback collection) could save staff time and deliver a more seamless experience to small business clients.</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Subject: Boosting Impact &amp; Efficiency for NJSBDC at Rutgers-Camden
+Hi [Name],
+I’m impressed by how NJSBDC @ Rutgers-Camden empowers South Jersey entrepreneurs with expert support and resources. We help nonprofit centers like yours streamline client engagement by automating appointment scheduling and intake forms, redesigning websites for easier resource access, and automating event follow-ups—freeing up staff for higher-impact work.
+Open to a quick call to explore how small automation wins can make a big difference for your team and the business owners you serve?</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ChIJgd3lOez5wokRPwdaAfANjsU</t>
+          <t>ChIJVQ1w2Mr9wokRrt2nYqXG4o0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Pompei Deli</t>
+          <t>NJSBDC at William Paterson University</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>gift_shop, point_of_interest, store, establishment</t>
+          <t>consultant, point_of_interest, establishment</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>(551) 221-7167</t>
+          <t>(973) 321-1378</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>4.8</v>
+        <v>4.6</v>
       </c>
       <c r="F3" t="n">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -582,64 +652,143 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>http://www.pompeigiftbaskets.com/</t>
+          <t>https://sbdcwpu.com/</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://maps.google.com/?cid=14235330796630705983&amp;g_mp=Cidnb29nbGUubWFwcy5wbGFjZXMudjEuUGxhY2VzLlNlYXJjaFRleHQQAhgEIAA</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">People say this gift basket store offers amazing, personalized gift baskets. They highlight the baskets are fully custom and beautifully arranged. They also like the fast shipping and helpful staff. </t>
-        </is>
-      </c>
+          <t>https://maps.google.com/?cid=10223952517711519150&amp;g_mp=Cidnb29nbGUubWFwcy5wbGFjZXMudjEuUGxhY2VzLlNlYXJjaFRleHQQAhgEIAA</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>I was recommended Pompei Gift Baskets by my friend and cannot continue to recommend them enough! They went above and beyond for my brother’s engagement bottle personalization. Daniela helped me and my mom out and was so kind through the whole process. Little requests I asked for were done which didn’t go unnoticed. She even rushed the order per my mom’s request. So kind and so helpful, love when I find family-owned business because it shows how dedicated they are to customer satisfaction. And pricing is EXCELLENT. Thank you! | Daniela and her family are the sweetest people who are so accommodating and are trying to give clients the best of the best! They work with you on customizing bottles with engravings and gift baskets that go above and beyond! Gaddi is a master at the engravings and really makes sure to get the right sizing and fonts for you. Highly recommend them and use them for all my gifting needs! | Why I love small businesses, and this one in particular!!
-Last week my team and I were on the search for the perfect gift for the perfect boss who has been under a lot of pressure.  We wanted to show her how much we appreciated her by getting her a gift basket.  Found this small company and was pleasantly surprised at the customization options for the basket. We placed the order for ground delivery at a great price.
-Shortly after booking, I got an email from Daniela letting me know there was an issue with the chocolates we selected and offered two great alternatives.  While they were making the basket, the found the wine option we selected had a crack. Once again she reached out and gave me the option to pick another bottle of higher value or wait a couple days for the new one to come in.  I was ok with waiting since she let me know it would make it before the following Saturday.
-To my surprise, the basket was expedited by Daniela and on a teams chat with the other leaders, our boss let us know she got the gift and broke down in excitement.  This gift reinvigorated her to conquer the rest of the week know she has a great wine to enjoy on Friday night!
-Special thanks to Daniela for the amazing communication and the beautiful gift package.
-You have a client for life now!</t>
+          <t>I cannot express enough gratitude for Dayna Caputo and her office for their incredible support in helping me complete my grant application for Merced Manor. As a small, women-owned business, navigating the grant process can be overwhelming, but Dayna’s patience, expertise, and unwavering support made all the difference. She guided me every step of the way, ensuring I had the resources and knowledge needed to succeed. This kind of support is tremendous for small businesses like mine, providing opportunities that can truly be transformative. Thank you, Dayna, for your dedication and for championing small business owners—you are making an invaluable impact! | I am so honored to have been a part of this amazing organization. Reina who is one of the mentors helped me by getting my certifications and my Google business up and running. I was with the organization for less than a year and won a SBDC Award, FedEx grant and got accepted into Target. For anyone who is looking for community and support, sign up today! They were all great! Thank you once again to everyone! | Extremely helpful for new start up businesses.  Very informative.</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>info@pompeigiftbaskets.com</t>
+          <t>sbdc@wpunj.edu</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>4.65</v>
+        <v>2.26</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>**UI Improvements:**
+1. **Above-the-Fold Content**:
+   - The top portion of the site is mostly empty space, which creates a weak first impression and forces users to scroll. Consider filling the hero section with a clear call-to-action, an engaging heading, or a hero image/graphic that communicates your brand message.
+2. **Branding &amp; Cohesiveness**:
+   - While the color palette is consistent, the pink overlay on images does not align well with the rest of the brand’s professional and clean navy/white look. Try subtler image overlays or use real, vibrant photos.
+3. **Navigation/Menu Bar**:
+   - The navigation bar font appears small and spaced far apart, which may make reading and targeting links difficult, especially on larger screens. Increase font size and padding for improved usability.
+   - The social media icons are minimally visible; increasing their size or changing color on hover would improve visibility.
+4. **Content Density and Balance**:
+   - The long scroll between the header and actual content sections (e.g., "Recent Events") feels unbalanced. Tighten up vertical spacing to make better use of screen real estate.
+   - The “Recent Events” module appears with a blank space below it, which is confusing. Either populate this area or remove the heading until events exist.
+5. **Accessibility**:
+   - While there’s an accessibility plugin/widget visible, some color contrast (like white text on red or yellow stars on navy) could be improved—especially for visually impaired users.
+   - Consider ensuring buttons and links are keyboard/tab accessible with visible focus indicators.
+6. **Modern UI Trends**:
+   - The large empty areas and blocks of color feel outdated; modern UIs use more white space strategically, layering, slight shadows, and gradients for depth.
+   - Card elements at the bottom could use soft drop shadows or slightly rounded corners for a more contemporary look.
+   - Consider using more visually engaging components like icons, illustrations, or animation for key interactions.
+7. **Form Design**:
+   - Newsletter sign-up fields (first/last name, email) lack clear labeling and inline validation. They could be arranged horizontally on wider screens for a more compact look.
+   - The “Submit” button design is very basic and easily missed—use a more prominent button with higher contrast or include an icon.
+8. **Image &amp; Content Overlays**:
+   - The colored overlays on images (deep red and blue) can obscure photo details, making the visuals less engaging. Use more subtle overlays and/or increase photo brightness.
+   - Sponsor section looks cohesive but could use more breathing room between logos to avoid a cramped feel.
+9. **Mobile Responsiveness**:
+   - While responsiveness can't be confirmed in a screenshot, large fixed-width sections and lots of horizontal cards can create problems on mobile. Make sure all cards stack vertically and padding/margins are mobile-friendly.
+10. **Hierarchy &amp; Typography**:
+    - Use more pronounced headings and subheadings to break up sections and guide the user's eye.
+    - Ensure consistent heading sizes and spacing for a polished appearance.
+---
+**Summary:**  
+The site communicates trust but feels slightly outdated and lacks visual engagement above the fold. Tighten spacing, modernize visuals (shadows, gradients, cards), improve above-the-fold content, revisit color/accessibility contrast, and use real imagery. Make navigation, forms, and CTAs more usable and visible. Adjust overlays for cleaner, more inviting branding. 
+**(Note: All suggestions are UI-focused and not about content/functionality.)**</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>### 1. Business Identity, Industry, and Positioning
+**Business:**  
+The New Jersey Small Business Development Center (NJSBDC) at William Paterson University
+**Industry:**  
+Business and economic development, focusing on small business support
+**Positioning:**  
+A publicly and privately funded resource hub offering no-cost counseling, education, training, and professional advice to small businesses and entrepreneurs in Passaic and Union counties, New Jersey. The center operates within William Paterson University’s Cotsakos College of Business and partners with the SBA and other organizations to help local businesses start, grow, and thrive.
+---
+### 2. Personalized Brief with Opportunities
+The NJSBDC at William Paterson University plays a critical role in empowering small business owners and entrepreneurs across northern New Jersey with no-cost expert counseling, business plan development, access to capital, networking, and training resources. Given the center’s wide-ranging service offerings and high community engagement, there are quick wins available through enhanced automation—such as streamlining appointment scheduling, intake, and follow-up processes (e.g., online booking, automated email reminders, and digital resource delivery). Modernizing the website for a more seamless navigation and accessibility experience, and integrating self-service tools (such as smart FAQs or resource libraries), could also improve client engagement and reduce manual workload. Additionally, mapping workflows for event promotion, sign-ups, and feedback collection could further optimize internal processes—amplifying the center’s already strong impact and freeing up time for deeper one-on-one advising and partnership development.</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>**Business Pain Point Report**  
+*Client: The New Jersey Small Business Development Center (NJSBDC) at William Paterson University*
+---
+**Pain Point 1: Outdated Website Design &amp; Suboptimal User Experience**  
+  - **Impact:** The website’s current design—with empty above-the-fold space, outdated visual elements, and weak CTAs—may create a poor first impression for new visitors. This can lead to lost engagement, lower trust, and reduced inquiries or event sign-ups, damaging credibility as a leading business resource.
+  - **How We Can Help:** *Website Redesign Services* – We will modernize your website for intuitive navigation, engaging visuals, improved CTAs, and consistent branding. Enhanced accessibility and responsive design will ensure all users, including those with disabilities or on mobile devices, can easily access your resources and connect with your team.
+---
+**Pain Point 2: Manual and Inefficient Operational Processes**  
+  - **Impact:** High client volume and diverse service offerings likely rely on manual steps for scheduling, intake, appointment reminders, event sign-ups, and follow-up. This wastes staff time, delays responses, increases the risk of dropped leads, and limits the center’s ability to scale support or increase counseling capacity.
+  - **How We Can Help:** *Process Automation (Operations &amp; Support)* – We will implement online appointment booking, automated intake questionnaires, triggered email reminders, self-service resource delivery, and automated feedback collection. This will reduce administrative workload and enable your consultants to invest more time in high-value advising.
+---
+**Pain Point 3: Limited Self-Service Digital Tools &amp; Knowledge Access**  
+  - **Impact:** The current website offers limited interactive features (e.g., no smart FAQ, resource libraries, or live chat). This means prospective clients with common questions must wait for a staff response, causing delays, increasing staff workload, and potentially deterring new sign-ups or follow-ups.
+  - **How We Can Help:** *Digital Self-Service Integration &amp; Consulting* – We’ll equip your site with smart knowledge bases, dynamic FAQs, and an accessible resource portal, plus chatbots for common inquiries. This empowers clients to find information instantly and allows staff to focus on complex or high-touch support.
+---
+**Pain Point 4: Lack of Workflow Mapping for Event Management &amp; Feedback**  
+  - **Impact:** Event promotion, registration, and feedback collection may be handled manually or with ad-hoc tools, leading to inconsistent outreach, lost registrations, potentially lower attendance, and missed insights on event effectiveness.
+  - **How We Can Help:** *Organizational/Process Consulting &amp; Event Automation* – We can map, document, and streamline your event workflows, integrating automated promotion, sign-up forms, and post-event feedback surveys. This boosts event success, reduces effort, and delivers actionable analytics for ongoing improvement.
+---
+**Pain Point 5: Potential Gaps in Financial Process Efficiency**  
+  - **Impact:** While not visible in the UI or reviews, the center supports small business finances and may itself benefit from streamlined, transparent bookkeeping and reporting—especially as partnerships and funding streams grow. Inefficient processes here could lead to missed grant/partnership opportunities or reporting bottlenecks, reducing organizational agility.
+  - **How We Can Help:** *Bookkeeping &amp; Accounting Services* – We’ll assess and optimize your internal financial tracking and reporting, using cloud-based tools for real-time insights, cleaner audits, and easier grant compliance. This enhances organizational professionalism and positions NJSBDC as a model for the clients it supports.
+---
+**Summary**  
+Your team’s reputation for supportive, transformative guidance is clear from stellar reviews. Modernizing your digital presence and automating key touchpoints will ensure NJSBDC’s operational excellence matches the passion of its staff—delivering even greater impact to New Jersey’s small business community. We look forward to supporting your next phase of growth.</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Subject: Elevate NJSBDC’s Impact with Seamless Digital Solutions
+Hi [Name],
+I’m impressed by NJSBDC at William Paterson’s dedication to empowering small businesses in Passaic and Union counties. We can help amplify your impact by modernizing your website for better accessibility and engagement, and automating manual workflows—like appointment scheduling and event sign-ups—so your team spends less time on admin and more on advising. We also offer tailored consulting to streamline event management and optimize feedback collection.
+Would you be open to a quick call next week to explore how we can support your mission?</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ChIJee4ElqX8wokRcOKryJ1sHTc</t>
+          <t>ChIJE94joD1RwokRaH_X2VXRENk</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Carrick Mor Irish Store Bergen County Glen Rock NJ</t>
+          <t>NJ Small Business Development Center at NJCU School of Business</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>gift_shop, point_of_interest, store, establishment</t>
+          <t>corporate_office, point_of_interest, establishment</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(201) 444-9230</t>
+          <t>(201) 200-2156</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>4.9</v>
+        <v>4.8</v>
       </c>
       <c r="F4" t="n">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -648,57 +797,152 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>http://www.carrickmor.com/#!contact/c24vq</t>
+          <t>https://www.sbdchudsoncounty.com/</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://maps.google.com/?cid=3971449871343018608&amp;g_mp=Cidnb29nbGUubWFwcy5wbGFjZXMudjEuUGxhY2VzLlNlYXJjaFRleHQQAhgEIAA</t>
+          <t>https://maps.google.com/?cid=15641231672514936680&amp;g_mp=Cidnb29nbGUubWFwcy5wbGFjZXMudjEuUGxhY2VzLlNlYXJjaFRleHQQAhgEIAA</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Carrick Mor Irish Store is such a special place! From the moment you walk in, you feel a sense of warmth and charm that’s hard to find anywhere else. The shop is filled with beautiful, authentic Irish items that you can tell were chosen carefully
-Mike, the owner, truly makes the experience unforgettable. He’s so kind, welcoming, and knowledgeable, and you can tell he genuinely cares about his customers and the community. He takes the time to share stories and build connections
-This isn’t just a store, it’s an experience one that leaves you feeling connected to Irish culture and tradition. If you’re looking for something unique, meaningful, or just want to be treated like family, Carrick Mor is the place to go. Thank you, Mike, for creating such a wonderful shop! | Cute Irish shop with authentic items from Ireland and more. | My wife and I have made numerous purchases here over the years, both online and in person. We have always been absolutely delighted with the quality of both the goods and the service received.   We especially appreciate the fact that the owners offer only tasteful goods that reflect the true pride and creativity of Ireland. We wish them every success in the years ahead.</t>
+          <t>Highly recommend! I took a couple workshops earlier this year that have helped tremendously. I took the course which assisted in establishing my llc and tax id creation and also the business plan work shop. Plenty of beneficial webinars are being offered even in the pandemic which is great. Grateful for these affordable resources as a new business owner! | They offer unbelievable and extremely resourceful courses for free for a  person to be inform and win at their business.  All personnel is well  educated, informed and wants to see you win.  Extremely helpful, knowledgeable and thoughtful counselors who guide you in the right direction as an entrepreneur  with no knowledge of business (but only the thought to win)!  There is no free help for those who want to excel at staring their own ventures and want everyone around them to shine as well, only this program! | I have attended many trainings with NJSDC.  The information I received was vital to me building the foundation for Stefanie Blue Consulting. They were knowledgeable in every aspect of business from finance to marketing and sales. Whether you are providing a service or selling a product the information covers every question you may have about starting a new business.  AND they make themselves available to you after the trainings.</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>info@carrickmor.com</t>
+          <t>sbdc@njcu.edu</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>4.15</v>
+        <v>2.19</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Here are the **UI improvements** identified for the website screenshot:
+---
+### **1. Outdated Visual Style**
+- The design does not follow the latest minimalistic and “clean” UI trends; it appears somewhat dated with heavy drop shadows, gradients, and dense content blocks.
+- There is a reliance on large, bold text rather than visual hierarchy and white space for emphasis.
+### **2. Inconsistent Branding &amp; Color Palette**
+- The palette is patriotic (red, white, blue), but the shades and saturation vary between sections, making the branding feel inconsistent.
+- The “Learn More” and “Register for Success” buttons use different tones of red.
+- Visual hierarchy between sections is muddled due to inconsistent background colors and call-to-action styles.
+### **3. Typography Issues**
+- Too many font weights, sizes, and colors create a cluttered look. For example, the mix of vibrant white/grey and bold fonts in headings is visually jarring.
+- Paragraphs are justified inconsistently and could benefit from more line spacing for improved readability.
+### **4. Layout &amp; Spacing**
+- There is not enough padding/space between many sections, leading to a crowded feeling.
+- The blocks for “Start”, “Grow”, “Expand” are the same width but could use more padding and less text, perhaps with icons to improve at-a-glance understanding.
+- The search field under “Training &amp; Events” is very squeezed and visually unbalanced.
+### **5. Accessibility/Usability**
+- Insufficient color contrast in some areas (light gray backgrounds with white or light text).
+- Some text blocks are hard to read due to size or lack of spacing.
+- Buttons could be larger and have a clearer focus state for keyboard navigation.
+- The placeholder text in the newsletter form is almost the same color as the background, reducing readability.
+### **6. Visual Consistency**
+- The navigation bar menu, popup, and search icon styles differ from the rest of the site.
+- The “Hey, Welcome!” section feels separated stylistically and lacks visual integration with the main brand.
+- Uneven use of drop shadows (e.g., behind the monitor mockup) feels inconsistent with flat, modern UI trends.
+### **7. Imagery**
+- Hero image is nice but low-contrast and doesn’t create a strong brand feeling; consider higher contrast or blended overlays for legibility.
+- Stock imagery (the computer monitor) doesn’t add value — custom or more relevant visuals would enhance credibility.
+### **8. Footer**
+- The footer area is dense with small text links; these could be made more readable and separated with increased line height or appropriate spacing.
+- Social icons lack enough padding and contrast for prominence.
+---
+## **Summary of Recommendations**
+- Adopt a more minimal, modern look with larger white spaces, flatter colors, and fewer font styles.
+- Use a cohesive color palette throughout; align all CTA buttons to a single style.
+- Increase spacing between sections and avoid crowding text blocks.
+- Ensure all text and UI components have sufficient contrast for accessibility.
+- Replace or remove outdated stock images; use consistent iconography.
+- Redesign the newsletter form for clarity and make input fields more prominent.
+- Refine the navigation and footer for better usability and user experience.
+---
+**Overall, the site is functional but feels outdated with several UI/UX practices that don’t align with modern web standards and accessibility trends.**</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>**Client Brief:**
+The Small Business Development Center (SBDC) at New Jersey City University is a non-profit, government-funded resource center supporting entrepreneurs and small business owners in Hudson County, New Jersey. They offer no-cost one-on-one counseling, training, and advisory services to help businesses start, grow, and expand, with expertise spanning access to capital, strategic planning, marketing, HR, and more. As a pivotal hub for local business education and support, SBDC could benefit from automating appointment booking, centralizing event and resource materials, and redesigning its website for easier navigation and mobile responsiveness. Streamlining intake and follow-up processes would also maximize their advisors’ impact, while improvements to the newsletter signup experience could boost community engagement and information dissemination.</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>**Business Pain Point Report**
+---
+### Pain Point 1: Outdated, Inconsistent, and Unintuitive Website Design  
+- **Impact:**  
+  The current user experience on the website is below modern standards, which can lead to visitor frustration, reduced engagement with resources, and difficulty accessing essential services. Potential clients might perceive the center as less progressive or trustworthy, potentially hurting sign-ups for counseling, workshops, and newsletters. Accessibility issues could also limit outreach to users with disabilities, while mobile unfriendliness hampers engagement from busy entrepreneurs on-the-go.
+- **How We Can Help:**  
+  *Website Redesign:* We offer a ground-up modernization of the website’s design, applying clean, accessible, and mobile-first UI/UX standards. This includes a unified color palette, strong visual hierarchy, optimal spacing, accessible elements, and cohesive branding to reinforce trust and credibility — ensuring a frictionless journey from landing page to user action.
+---
+### Pain Point 2: Manual/Fragmented Operations for Appointment Booking and Intake  
+- **Impact:**  
+  Manual or unintegrated processes for appointment scheduling, client onboarding, and post-session follow-up are prone to errors and bottlenecks, absorbing valuable staff and advisor time. This diminishes the center’s capacity to serve more clients, causes potential lost opportunities, and slows the overall client journey.
+- **How We Can Help:**  
+  *Automation of Operations:* We can implement secure, user-friendly automation solutions for appointment booking, intake forms, and follow-up communications. By centralizing and digitizing these workflows, the SBDC will save staff hours, increase scheduling accuracy, and provide a seamless experience for clients from first point of contact through ongoing support.
+---
+### Pain Point 3: Disjointed Access to Resource Materials, Training Events, and Newsletters  
+- **Impact:**  
+  Valuable information is harder for entrepreneurs to find or access, resulting in lower event attendance, missed opportunities for education, and underutilization of available resources. A confusing or cumbersome newsletter signup process reduces engagement and diminishes the center’s ability to inform and mobilize its community.
+- **How We Can Help:**  
+  *Process Consulting &amp; Website Integration:* We will streamline the website’s resource center, event management, and newsletter functions. This includes developing a centralized resource hub, improving filtering/search for trainings, and revamping the newsletter signup for maximum visibility and ease. These changes help boost participation rates, make knowledge more accessible, and deepen ongoing relationships with the small business community.
+---
+### Pain Point 4: Inconsistent Branding and Weak Visual Identity Online  
+- **Impact:**  
+  Variability in color schemes, button styles, and iconography can dilute brand recognition and reduce the perceived professionalism of the organization. This weakens emotional connection and makes it harder for SBDC to stand out as a leader and trusted adviser in the eyes of local entrepreneurs and partners.
+- **How We Can Help:**  
+  *Brand Alignment Through Redesign:* Our team can audit and unify the digital visual identity, creating a style guide that ensures consistent branding, tone, and usability across web pages and communication channels. A modern, reliable look increases trust, strengthens your brand in the minds of visitors, and supports organizational growth.
+---
+### Pain Point 5: Lack of Systematic Measurement and Continuous Improvement  
+- **Impact:**  
+  Without integrated digital touchpoints and reporting, gauging the effectiveness of outreach initiatives and client engagement efforts is difficult. Missing or incomplete data can result in missed opportunities to improve or expand high-impact services, and hinders reporting to funders or stakeholders.
+- **How We Can Help:**  
+  *Automation &amp; Analytics Integration:* We can enable website and process automation with built-in analytics — tracking sign-ups, resource downloads, event participation and more. This data will empower leadership to make informed decisions, optimize programs, and demonstrate value to funders and partners.
+---
+**Summary for Outreach:**  
+While SBDC at NJCU is highly valued by its community, there is substantial opportunity to multiply its impact through modernization of its online presence, automation of staff-intensive processes, and integration of central resources. Our proven expertise can help SBDC streamline operations, improve client and staff experience, and strengthen the organization’s standing as a forward-looking pillar for New Jersey’s small businesses.</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Subject: Unlock Greater Impact for SBDC at NJCU
+Hi [Name],
+I’m impressed by the SBDC’s commitment to Hudson County’s entrepreneurs, but I noticed the website and intake process could be holding your team back. A modern, mobile-friendly redesign and automated booking system would help your advisors serve more small businesses—while a streamlined resource and event hub boosts community engagement. Are you open to a quick call to discuss how we can help SBDC deliver even greater impact?</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ChIJS1cVwT3lwokRGDrcldGHDAg</t>
+          <t>ChIJaQ76833iwokRVpua7_cM-M4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>The Gift Shoppe at Curbside Confections</t>
+          <t>PROFESSIONAL BUSINESS STRATEGIES, LLC</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>gift_shop, point_of_interest, store, establishment</t>
+          <t>consultant, point_of_interest, establishment</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>(201) 986-6511</t>
+          <t>(201) 425-8300</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4.6</v>
       </c>
       <c r="F5" t="n">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -707,86 +951,133 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>http://curbsideconfections.com/giftshoppe</t>
+          <t>http://www.pbstrategies.com/?utm_source=google&amp;utm_medium=wix_google_business_profile&amp;utm_campaign=10151791167836211045</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://maps.google.com/?cid=579987786256103960&amp;g_mp=Cidnb29nbGUubWFwcy5wbGFjZXMudjEuUGxhY2VzLlNlYXJjaFRleHQQAhgEIAA</t>
+          <t>https://maps.google.com/?cid=14913684425053739862&amp;g_mp=Cidnb29nbGUubWFwcy5wbGFjZXMudjEuUGxhY2VzLlNlYXJjaFRleHQQAhgEIAA</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t>The Gift Shoppe is absolutely amazing! Aside from the beautiful, brand-new interior, they have so many unique toys and candy to take a look at. They also have partnered with local Party With Sol and host exquisite parties on the second floor of the Gift Shoppe. From building your own bear to making custom bracelets, the parties are wonderful! I highly recommend having your next party on the second floor of Curbside Confection's Gift Shoppe! | What a spectacular Gift Shoppe! Curbside confections has something for everyone. The displays are gorgeous, showcasing unique gift ideas, sweets, toys, classic candy favorites and the variety of taffy flavors are enough to make any mouth water.  One of my favorite takeaways are the "Handy Chops" chop sticks with a fun twist.
-May I suggest the chocolate covered gummed bears? You won't be sorry. So Goood!!
-Im so glad we stopped in while we were in town. A special thanks to Tyler for sharing his favorites. They did not disappoint 😉. | Cannot recommend this venue enough. Amazing staff, personalized  service and made everything so easy from start to finish. Thank you for an awesome event and making my daughter’s birthday so special!</t>
+          <t>I'm thrilled to share my 5-star experience with Dennis Bonagura! Over the past 5 years, Dennis has been an instrumental partner in my business journey, guiding me from $100,000 in my first year to $1.7 million in annual revenue (year 5). What sets Dennis apart is not just his exceptional business expertise, but his genuine care and mentorship. He's more than just my coach - he's a trusted friend and advisor who's always there to offer me valuable insights, celebrate successes, and provide guidance during challenging times.
+Dennis has a unique ability to pinpoint areas for improvement and highlight strengths, providing actionable advice that drives results. His strategies are practical, and his support is unwavering. I highly recommend Dennis to anyone seeking a beneficial business coach who can offer a fair and affordable guidance, as well as a trusted partner to navigate both triumphs and setbacks with.
+5 stars isn't enough - Dennis has truly transformed my business and my whole life!
+David Peers
+President
+Cutting Edge Consulting Group Inc. | Great experience working with PBS.  Dennis has had a huge impact on the success of my plumbing &amp; heating company.
+He has certainly brought CLARITY to WHAT MATTERS MOST!! | Professional Business Strategies is a truly a forward thinking firm due to their knowledge and experience in dealing with today's complicated workplace.
+I've known Dennis Bonagura for years but it wasn't until I was unemployed that I truly learned of the great business sense he fostered in personal development.  He looked at my resume which was professionally done and in his charming way said it wasn't what today's hiring manager was looking for in the 45 seconds they'd spend on the first glance!  He advised the changes that I should make and to transfer that to my LinkedIn profile as well.  I started receiving more hits immediately and was back to work within a month.
+I take great pleasure thanking Dennis every time I see him!
+John McCauley
+Senior Project Manager
+Global Banking Liquidity Regulations</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>info@curbsideconfections.com, giftshoppe@curbsideconfections.com, party@curbsideconfections.com</t>
+          <t>dbonagura@pbstrategies.com</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>4.19</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ChIJg7rhwlL6wokRl9s1UISX-iY</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>3D innovation - Customized &amp; Personalized Gifts, Memorials &amp; Awards - Paramus, NJ</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>gift_shop, home_goods_store, point_of_interest, store, establishment</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>(201) 226-0021</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="F6" t="n">
-        <v>41</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>OPERATIONAL</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>https://3dinnovation.com/NJ</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>https://maps.google.com/?cid=2808723912156109719&amp;g_mp=Cidnb29nbGUubWFwcy5wbGFjZXMudjEuUGxhY2VzLlNlYXJjaFRleHQQAhgEIAA</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Turn that great photo into a truely amazing 3D crystal likeness. Excellent gift idea for Mothers day, weddings, anniversary or some other special occasion. It's also a good gift for someone who has everything. The help are friendly in this kiosk near the Pink store on the lower level. | I must tell you this memorial gift from a friend was the most beautiful keepsake to cherish. I loved the crystal heart etched with my parents images so much that I decided to give one to each of my sisters. Melany was so wonderful to work with and she had the artwork on file and duplicated the keepsake for both of my sisters ...shipped them to me within a week. Melany was so sweet and caring and just a dream to work with. Although I'm several states away I will contact Melany to work with in the future!!! | I had an issue with the brightness of the crystal that I purchased. Luckily, Mel provided me with amazing service. She listened to the request I made and immediately fixed the brightness of the crystal in a very professional way. Mel's personality and professionalism earned them a returning customer.</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>info@3d-innovation.com</t>
-        </is>
-      </c>
-      <c r="M6" t="n">
-        <v>3.91</v>
+        <v>2.2</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>**UI Improvements:**
+1. **Outdated Visual Style:**
+   - The website’s design feels dated, lacking the modern minimalism and polish seen in contemporary websites (e.g., more whitespace, card-based layouts, subtle gradients).
+   - Blurred stock images are overused and detract from visual appeal and clarity. Modern websites favor high-quality or brand-specific imagery.
+2. **Brand Cohesion:**
+   - The logo and color scheme (black, blue, and white) are consistent, but the imagery does not reinforce the brand identity. More customized or on-brand images would help.
+   - Font usage is not distinctive or modern; incorporating a unique, legible typeface can help with brand recognition.
+3. **Layout &amp; Spacing:**
+   - Content sections are very dense, especially in mobile view. Add more padding/spacing between sections and content blocks for readability and visual ease.
+   - The contact form abruptly changes to a stark white background, breaking the visual flow. Maintain consistent background color or subtle separator.
+4. **Typography:**
+   - Font sizes for body and header text lack hierarchy. Use larger headings, more pronounced subheadings, and balanced body text for easier scanning.
+   - Text over images lacks sufficient contrast, especially in the hero section (white text on a bright image). Apply overlays or darker image filters to increase readability.
+5. **Images &amp; Visuals:**
+   - Repeated blurry images dilute professionalism; use sharp, high-res images or subtle illustrations/icons that match the brand’s message.
+   - Consider modern design elements such as soft drop shadows, rounded corners, or micro-animations for buttons and images.
+6. **Buttons &amp; Calls-to-Action:**
+   - "Read More" buttons are generic; use more descriptive labels to guide users (e.g., "Explore Services," "View Assessment Details").
+   - Buttons lack visual emphasis (size/color/shape); make them stand out more with contrast and subtle animation.
+7. **Accessibility:**
+   - Text contrast (especially text over images) is insufficient for accessibility. Use WCAG-compliant contrast ratios.
+   - Navigation/text size and button elements should be larger/more touch-friendly on mobile.
+   - Consider skip navigation and ARIA roles for improved accessibility.
+8. **Footer:**
+   - The footer feels disconnected; increase padding, organize links into columns, and use icons for social media.
+   - The use of three very different background colors (black, white, blue) hampers cohesion. Unify backgrounds for a smoother flow.
+9. **Usability:**
+   - Add sticky/fixed navigation for easier access to sections.
+   - The testimonials section should use consistent card heights and consider a carousel/slider for modern presentation.
+10. **Modern Trends:**
+    - Add subtle animations or transitions to images/buttons for a modern touch.
+    - Integrate subtle gradients or glassmorphism as a background or highlight to catch up with current UI trends.
+---
+**Summary:**  
+While the website has a clear structure and basic cohesion, it requires significant modernization in imagery, visual flow, accessibility, and interactivity to compete with current UI/UX standards and produce a more polished, professional experience.</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>**Client Brief:**
+Professional Business Strategies, LLC, led by Dennis Bonagura in Bergen County, NJ, is a business coaching and consulting firm specializing in supporting business owners, executives, and sales professionals. Dennis is a Certified Professional Business Coach with over 30 years' leadership experience, offering tailored coaching, executive mentoring, sales team development, and behavioral assessments (Extended DISC®) to help clients gain clarity, improve performance, and resolve common organizational challenges like stagnant sales, profitability, and staff turnover. Quick wins could include automating appointment scheduling and assessment delivery, revamping the website for cleaner navigation and clearer calls-to-action (e.g., "Book a Free Strategy Session"), and systematizing recurring client feedback requests. Given the strong focus on clarity and actionable strategies, an operations/process audit could further identify bottlenecks in client onboarding or follow-up, while targeted web updates would reinforce their expert positioning and enhance lead capture.</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>**Business Pain Point Report**  
+*For Professional Business Strategies, LLC (PBS) – Dennis Bonagura*
+---
+**Pain Point 1: Outdated Website Design and User Experience**  
+- **Impact:**  
+  The website feels outdated and lacks modern polish, with issues in imagery, typography, spacing, contrast, calls-to-action, and accessibility. This risks undermining the firm’s credibility, deterring potential clients, and reducing conversion rates for key goals (e.g., booking strategy sessions or assessments). The lack of modern design and accessibility can make PBS appear less relevant or professional compared to competitors, impacting lead generation and first impressions.
+- **How We Can Help:**  
+  **Website Redesign:** Our web development team will implement a modern, brand-cohesive, and accessible redesign—utilizing high-quality images, improved typography, consistent branding, clear navigation, and engaging calls-to-action (e.g., “Book a Free Strategy Session”). Updates will make the website mobile-friendly, visually appealing, and optimized for lead capture, reinforcing PBS’s expert positioning and supporting business growth.
+---
+**Pain Point 2: Inefficient and Manual Business Processes**  
+- **Impact:**  
+  Recurring administrative tasks such as appointment scheduling, assessment delivery, and client feedback requests are likely handled manually, creating operational bottlenecks, wasting staff time, increasing error risk, and slowing down client onboarding or follow-up. This inefficiency can undermine the personalized coaching experience that Dennis offers, restrict capacity for growth, and frustrate clients expecting a seamless, modern experience.
+- **How We Can Help:**  
+  **Business Process Automation:** We can automate key workflows—including client scheduling, assessment/report delivery, client feedback collection, and routine communication—using platforms like Calendly, Zapier, or custom automation. This saves time, reduces human error, creates a smoother client journey, and allows Dennis to focus on value-adding work rather than repetitive tasks.
+---
+**Pain Point 3: Limited Systematic Approach to Collecting and Leveraging Client Feedback**  
+- **Impact:**  
+  While reviews indicate high satisfaction, feedback collection seems ad hoc. Lack of a systematic process can mean missed insights for business development, less social proof on digital channels, and an underutilization of client advocacy for marketing. This results in fewer compelling testimonials and a weaker demonstration of the firm’s impact to prospective clients.
+- **How We Can Help:**  
+  **Organizational/Process Consulting:** We’ll develop a structured feedback process—automating regular follow-up requests for testimonials, Net Promoter Score (NPS), and surveying clients at key milestones. This not only increases the volume of valuable client feedback to display on the revamped website and marketing materials, but also provides Dennis with actionable insights to refine service delivery.
+---
+**Pain Point 4: Under-optimized Lead Generation and Conversion Funnel**  
+- **Impact:**  
+  Generic buttons, unclear calls-to-action, lack of lead magnets (like free strategy sessions), and a non-distinctive brand presence on the website may lead to missed opportunities to capture interest and qualify leads. This directly impacts the sales pipeline, lowering the number of quality leads and making marketing spend less effective.
+- **How We Can Help:**  
+  **Sales Operations Automation &amp; Strategic Website Updates:** We’ll optimize calls-to-action (CTAs), create compelling lead magnets (e.g., assessment previews, strategy session bookings), and systematize lead capture with integrated forms and CRM syncing. This ensures that website visitors are more likely to engage, book sessions, and enter the sales pipeline—improving both conversion rates and ROI from digital traffic.
+---
+**Pain Point 5: Untapped Opportunities in Financial and Operational Data Reporting**  
+- **Impact:**  
+  While the reviews highlight exceptional coaching results, there’s no mention of structured tracking/reporting on client or internal KPIs, financial metrics, or operational performance. Without this, the company may be missing insights for driving profitability, optimizing service delivery, or communicating value to clients in tangible ways.
+- **How We Can Help:**  
+  **Bookkeeping &amp; Performance Dashboard Setup:** Our team can implement streamlined bookkeeping and financial reporting, as well as dashboards for tracking key business and client metrics (growth, engagement, satisfaction). This enables more informed strategic decisions for PBS and enhances the firm’s ability to demonstrate client ROI in future engagements.
+---
+**Summary:**  
+Professional Business Strategies, LLC is well regarded for personalized, result-driven coaching, but faces clear pain points in web presence, process efficiency, systematic client feedback, lead generation, and data-driven operations. We recommend starting with a comprehensive website redesign and key process automations, followed by optimization of feedback and lead engagement processes, and support in financial reporting for maximum business impact.
+---</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Subject: Quick Wins for PBS: Website, Automation &amp; Growth
+Hi Dennis,  
+I’m impressed by your impact with PBS helping leaders in Bergen County, but noticed your website and workflow could be holding you back. A modern site redesign with clearer calls-to-action can boost credibility and lead capture, while automating tasks like scheduling and assessment delivery will free up your time for clients—not admin. I can also help you systematize feedback collection to showcase your success and drive growth.  
+Would you be open to a quick call next week to discuss actionable improvements?  
+Best,  
+[Your Name]</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>